<commit_message>
Minor mod to template
</commit_message>
<xml_diff>
--- a/data/OPenn_imagelist_template.xlsx
+++ b/data/OPenn_imagelist_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/RBS2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/Collation/github/VisColl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,6 +618,10 @@
     <row r="3" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="D3" s="1"/>
+      <c r="H3">
+        <f>H2+1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>

</xml_diff>

<commit_message>
minor mods to template
</commit_message>
<xml_diff>
--- a/data/OPenn_imagelist_template.xlsx
+++ b/data/OPenn_imagelist_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="16180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="38240" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Image URLs" sheetId="1" r:id="rId1"/>
@@ -6698,9 +6698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L686"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28326,7 +28324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2193" workbookViewId="0">
+    <sheetView zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B2223"/>
     </sheetView>
   </sheetViews>

</xml_diff>